<commit_message>
Work done with Rare Candy simulation
</commit_message>
<xml_diff>
--- a/src/WrittenWorks/ExcelSheetWork/PokemonProbabilities.xlsx
+++ b/src/WrittenWorks/ExcelSheetWork/PokemonProbabilities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcti\IdeaProjects\ProbabilityandAppliedStatistics\src\WrittenWorks\ExcelSheetWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E4578A-D038-4AD2-A7E3-85BA0A14033A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09CD92A-0411-4799-95F0-570F17627375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{D91CE332-9758-4AFE-B17D-4E873759518A}"/>
   </bookViews>
@@ -928,11 +928,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Comparison</a:t>
+              <a:t>Rare</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of Candies in Deck and Amount of Hands with Candies</a:t>
+              <a:t> Candy Counts vs. Hands with Candies</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -974,12 +974,12 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -990,21 +990,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Rare Candy Data'!$A$1:$A$4</c:f>
+              <c:f>'Rare Candy Data'!$B$1:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>118</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>111</c:v>
+                  <c:v>10.62</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104</c:v>
+                  <c:v>19.59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>121</c:v>
+                  <c:v>29.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,7 +1012,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3C9A-4D28-9526-9FD8D849B759}"/>
+              <c16:uniqueId val="{00000001-A67D-42CE-9C06-DC0BC292A931}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1025,18 +1025,18 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="305244383"/>
-        <c:axId val="64892079"/>
+        <c:axId val="810757392"/>
+        <c:axId val="810761712"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:idx val="0"/>
+                <c:order val="0"/>
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -1050,7 +1050,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Rare Candy Data'!$B$1:$B$4</c15:sqref>
+                          <c15:sqref>'Rare Candy Data'!$A$1:$A$4</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1058,16 +1058,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>99.882000000000005</c:v>
+                        <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>99.888999999999996</c:v>
+                        <c:v>2</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>99.896000000000001</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>99.879000000000005</c:v>
+                        <c:v>4</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1075,7 +1075,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-3C9A-4D28-9526-9FD8D849B759}"/>
+                    <c16:uniqueId val="{00000000-A67D-42CE-9C06-DC0BC292A931}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1084,7 +1084,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="305244383"/>
+        <c:axId val="810757392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1115,7 +1115,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Candies</a:t>
+                  <a:t> of Rare Candies in Deck</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -1186,7 +1186,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64892079"/>
+        <c:crossAx val="810761712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1194,7 +1194,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64892079"/>
+        <c:axId val="810761712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,12 +1239,20 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Hands with Candies</a:t>
+                  <a:t> of Hands with Rare Candies (%)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.9444444444444445E-2"/>
+              <c:y val="0.11152777777777778"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1305,7 +1313,485 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="305244383"/>
+        <c:crossAx val="810757392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Rare</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Candy Counts vs. Bricked Deck Chances</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Rare Candy Data'!$E$1:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.569999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AB2E-4F8A-BB07-428FFCEA7E1B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="957759231"/>
+        <c:axId val="957762591"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Rare Candy Data'!$D$1:$D$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-AB2E-4F8A-BB07-428FFCEA7E1B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="957759231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Rare Candies in Deck</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="957762591"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="957762591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="105"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Chance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Not Getting a Bricked Deck (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0555555555555555E-2"/>
+              <c:y val="0.14856481481481484"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="957759231"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1441,6 +1927,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1958,6 +2484,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2520,23 +3562,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>168275</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>307975</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92F7812F-B584-2481-0DE3-8430E3A17A40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C21E812-93B7-DC02-4D82-7D4F71B195FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2552,6 +3594,165 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DECB967-B8E1-D7A6-C885-9E614729E2BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Arrow: Bent-Up 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0565843-4A32-E8C9-6E63-6823532C5651}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="577850" y="831850"/>
+          <a:ext cx="349250" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentUpArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Arrow: Bent-Up 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9241165-DCBE-C088-7130-1C58EF7F33D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3117850" y="323850"/>
+          <a:ext cx="5060950" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentUpArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3363,44 +4564,68 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BD6E2F-62CC-4D38-98B8-AD23A65DA9AB}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>118</v>
+        <v>1</v>
       </c>
       <c r="B1">
-        <v>99.882000000000005</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>99.888999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>10.62</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>89.38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>104</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>99.896000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>19.59</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>80.41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>121</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>99.879000000000005</v>
+        <v>29.43</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>70.569999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>